<commit_message>
Update data to 2023
</commit_message>
<xml_diff>
--- a/input/spri_topics.xlsx
+++ b/input/spri_topics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haral\Documents\GitHub\globaltrends_spri\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c4361369\Documents\GitHub\globaltrends_spri\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2045B1D-7EDC-40A5-A95F-2698DED254D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D223D7B4-DAD0-4F94-B47D-2375E48934FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13515" activeTab="1" xr2:uid="{10DCA323-7FCA-4127-8054-0B27B40AD918}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20712" windowHeight="13512" xr2:uid="{10DCA323-7FCA-4127-8054-0B27B40AD918}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,17 +24,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -57,297 +46,153 @@
     <t>YouTube</t>
   </si>
   <si>
-    <t>%2Fm%2F02q_bk</t>
-  </si>
-  <si>
-    <t>%2Fm%2F055t58</t>
-  </si>
-  <si>
-    <t>%2Fm%2F025sndk</t>
-  </si>
-  <si>
-    <t>%2Fm%2F0d07ph</t>
-  </si>
-  <si>
-    <t>%2Fm%2F09jcvs</t>
-  </si>
-  <si>
     <t>Economy</t>
   </si>
   <si>
     <t>energy policy</t>
   </si>
   <si>
-    <t>%2Fm%2F04_wkd</t>
-  </si>
-  <si>
     <t>expropriation</t>
   </si>
   <si>
-    <t>%2Fm%2F0127bq</t>
-  </si>
-  <si>
     <t>nationalization</t>
   </si>
   <si>
-    <t>%2Fm%2F042px7</t>
-  </si>
-  <si>
     <t>trade policy</t>
   </si>
   <si>
     <t>economic growth</t>
   </si>
   <si>
-    <t>%2Fm%2F012_3l</t>
-  </si>
-  <si>
     <t>economy</t>
   </si>
   <si>
-    <t>%2Fm%2F0gfps3</t>
-  </si>
-  <si>
     <t>economic crisis</t>
   </si>
   <si>
-    <t>%2Fg%2F1211cg58</t>
-  </si>
-  <si>
     <t>stock market</t>
   </si>
   <si>
-    <t>%2Fm%2F0drqp</t>
-  </si>
-  <si>
     <t>Fiscal policy</t>
   </si>
   <si>
     <t>austerity</t>
   </si>
   <si>
-    <t>%2Fm%2F032qyr</t>
-  </si>
-  <si>
     <t>budget</t>
   </si>
   <si>
-    <t>%2Fg%2F120jxn0b</t>
-  </si>
-  <si>
     <t>debt</t>
   </si>
   <si>
-    <t>%2Fm%2F013y7y</t>
-  </si>
-  <si>
     <t>budget deficit</t>
   </si>
   <si>
-    <t>%2Fm%2F01nnwy</t>
-  </si>
-  <si>
     <t>fiscal policy</t>
   </si>
   <si>
-    <t>%2Fm%2F0z_xz</t>
-  </si>
-  <si>
     <t>stimulus</t>
   </si>
   <si>
-    <t>%2Fm%2F05q6c7n</t>
-  </si>
-  <si>
     <t>government spending</t>
   </si>
   <si>
-    <t>%2Fm%2F04g_71</t>
-  </si>
-  <si>
     <t>moratorium</t>
   </si>
   <si>
-    <t>%2Fm%2F04zwh1c</t>
-  </si>
-  <si>
     <t>tax</t>
   </si>
   <si>
-    <t>%2Fm%2F07g82</t>
-  </si>
-  <si>
     <t>Labor policy</t>
   </si>
   <si>
     <t>collective bargaining</t>
   </si>
   <si>
-    <t>%2Fm%2F01llkn</t>
-  </si>
-  <si>
     <t>jobs</t>
   </si>
   <si>
-    <t>%2Fg%2F122h6md7</t>
-  </si>
-  <si>
     <t>labor market</t>
   </si>
   <si>
-    <t>%2Fm%2F0nbdkp6</t>
-  </si>
-  <si>
     <t>minimum wage</t>
   </si>
   <si>
-    <t>%2Fm%2F04rsd</t>
-  </si>
-  <si>
     <t>unemployment</t>
   </si>
   <si>
-    <t>%2Fm%2F07s_c</t>
-  </si>
-  <si>
     <t>labor union</t>
   </si>
   <si>
-    <t>%2Fm%2F04gny</t>
-  </si>
-  <si>
     <t>Monetary policy</t>
   </si>
   <si>
     <t>central bank</t>
   </si>
   <si>
-    <t>%2Fm%2F01q82</t>
-  </si>
-  <si>
     <t>currency</t>
   </si>
   <si>
-    <t>%2Fm%2F01q7l</t>
-  </si>
-  <si>
     <t>exchange rate</t>
   </si>
   <si>
-    <t>%2Fm%2F018m33</t>
-  </si>
-  <si>
     <t>inflation</t>
   </si>
   <si>
-    <t>%2Fm%2F09jx2</t>
-  </si>
-  <si>
     <t>interest rate</t>
   </si>
   <si>
-    <t>%2Fm%2F04n7dpf</t>
-  </si>
-  <si>
     <t>monetary policy</t>
   </si>
   <si>
-    <t>%2Fm%2F01rd35</t>
-  </si>
-  <si>
     <t>money supply</t>
   </si>
   <si>
-    <t>%2Fm%2F016ldw</t>
-  </si>
-  <si>
     <t>Regulation</t>
   </si>
   <si>
     <t>dumping</t>
   </si>
   <si>
-    <t>%2Fm%2F01l28h</t>
-  </si>
-  <si>
     <t>banking supervision</t>
   </si>
   <si>
-    <t>%2Fg%2F121rjn4x</t>
-  </si>
-  <si>
     <t>black market</t>
   </si>
   <si>
-    <t>%2Fm%2F04rdmz</t>
-  </si>
-  <si>
     <t>competition law</t>
   </si>
   <si>
-    <t>%2Fm%2F0mxcs</t>
-  </si>
-  <si>
     <t>copyright</t>
   </si>
   <si>
-    <t>%2Fm%2F0h6sm4</t>
-  </si>
-  <si>
     <t>deposit insurance</t>
   </si>
   <si>
-    <t>%2Fm%2F05lkwy</t>
-  </si>
-  <si>
     <t>monopoly</t>
   </si>
   <si>
-    <t>%2Fm%2F04rwd</t>
-  </si>
-  <si>
     <t>patent</t>
   </si>
   <si>
-    <t>%2Fm%2F05sq5</t>
-  </si>
-  <si>
     <t>price fixing</t>
   </si>
   <si>
-    <t>%2Fm%2F0mxd7</t>
-  </si>
-  <si>
     <t>regulation</t>
   </si>
   <si>
-    <t>%2Fm%2F013zzb</t>
-  </si>
-  <si>
     <t>Trade policy</t>
   </si>
   <si>
     <t>protectionism</t>
   </si>
   <si>
-    <t>%2Fm%2F013z93</t>
-  </si>
-  <si>
     <t>tariff</t>
   </si>
   <si>
-    <t>%2Fm%2F0ffnx</t>
-  </si>
-  <si>
-    <t>%2Fm%2F0bhbmdc</t>
-  </si>
-  <si>
     <t>trade treaty</t>
   </si>
   <si>
-    <t>%2Fm%2F01fsk5</t>
-  </si>
-  <si>
     <t>Government</t>
   </si>
   <si>
@@ -357,150 +202,81 @@
     <t>authoritarian</t>
   </si>
   <si>
-    <t>%2Fm%2F014zf</t>
-  </si>
-  <si>
     <t>autocracy</t>
   </si>
   <si>
-    <t>%2Fm%2F0d8tn</t>
-  </si>
-  <si>
     <t>dictator</t>
   </si>
   <si>
-    <t>%2Fm%2F02bms</t>
-  </si>
-  <si>
     <t>fascism</t>
   </si>
   <si>
-    <t>%2Fm%2F02zmm</t>
-  </si>
-  <si>
     <t>military regime</t>
   </si>
   <si>
-    <t>%2Fg%2F11c5s_rnxq</t>
-  </si>
-  <si>
     <t>political oppression</t>
   </si>
   <si>
-    <t>%2Fm%2F04qwqn</t>
-  </si>
-  <si>
     <t>political prisoner</t>
   </si>
   <si>
-    <t>%2Fm%2F099cd</t>
-  </si>
-  <si>
     <t>prosecution</t>
   </si>
   <si>
-    <t>%2Fm%2F017tz9</t>
-  </si>
-  <si>
     <t>Corruption</t>
   </si>
   <si>
     <t>bribe</t>
   </si>
   <si>
-    <t>%2Fm%2F01mq8p</t>
-  </si>
-  <si>
     <t>bureaucracy</t>
   </si>
   <si>
-    <t>%2Fm%2F01g_y</t>
-  </si>
-  <si>
     <t>corruption</t>
   </si>
   <si>
-    <t>%2Fm%2F09pngm</t>
-  </si>
-  <si>
     <t>welfare reform</t>
   </si>
   <si>
-    <t>%2Fg%2F121zc50z</t>
-  </si>
-  <si>
     <t>government</t>
   </si>
   <si>
-    <t>%2Fm%2F036nz</t>
-  </si>
-  <si>
     <t>political party</t>
   </si>
   <si>
-    <t>%2Fm%2F05_5d</t>
-  </si>
-  <si>
     <t>politics</t>
   </si>
   <si>
-    <t>%2Fm%2F05qt0</t>
-  </si>
-  <si>
     <t>Rule of law</t>
   </si>
   <si>
     <t>court</t>
   </si>
   <si>
-    <t>%2Fm%2F0k05r</t>
-  </si>
-  <si>
     <t>nepotism</t>
   </si>
   <si>
-    <t>%2Fm%2F01tj9r</t>
-  </si>
-  <si>
     <t>Stability</t>
   </si>
   <si>
     <t>candidate</t>
   </si>
   <si>
-    <t>%2Fm%2F02wwvy</t>
-  </si>
-  <si>
     <t>coup d'etat</t>
   </si>
   <si>
-    <t>%2Fm%2F025k7</t>
-  </si>
-  <si>
     <t>election</t>
   </si>
   <si>
-    <t>%2Fm%2F02l3h</t>
-  </si>
-  <si>
     <t>impeachment</t>
   </si>
   <si>
-    <t>%2Fm%2F03yr9</t>
-  </si>
-  <si>
     <t>opposition</t>
   </si>
   <si>
-    <t>%2Fm%2F098j6v</t>
-  </si>
-  <si>
     <t>vote</t>
   </si>
   <si>
-    <t>%2Fm%2F0pgkc</t>
-  </si>
-  <si>
     <t>Security</t>
   </si>
   <si>
@@ -510,180 +286,96 @@
     <t>military</t>
   </si>
   <si>
-    <t>%2Fm%2F01h6rj</t>
-  </si>
-  <si>
     <t>blockade</t>
   </si>
   <si>
-    <t>%2Fm%2F01qvj2</t>
-  </si>
-  <si>
     <t>embargo</t>
   </si>
   <si>
-    <t>%2Fg%2F1218dzhd</t>
-  </si>
-  <si>
     <t>attack</t>
   </si>
   <si>
-    <t>%2Fg%2F1q6j9fx10</t>
-  </si>
-  <si>
     <t>sanctions</t>
   </si>
   <si>
-    <t>%2Fm%2F06mz9c</t>
-  </si>
-  <si>
     <t>war</t>
   </si>
   <si>
-    <t>%2Fm%2F082cb</t>
-  </si>
-  <si>
     <t>Internal</t>
   </si>
   <si>
     <t>fundamentalism</t>
   </si>
   <si>
-    <t>%2Fm%2F032b8</t>
-  </si>
-  <si>
     <t>independence</t>
   </si>
   <si>
-    <t>%2Fm%2F0gwb1</t>
-  </si>
-  <si>
     <t>martial law</t>
   </si>
   <si>
-    <t>%2Fm%2F0dbs_</t>
-  </si>
-  <si>
     <t>militia</t>
   </si>
   <si>
-    <t>%2Fm%2F055sg</t>
-  </si>
-  <si>
     <t>protest</t>
   </si>
   <si>
-    <t>%2Fg%2F120ry1nd</t>
-  </si>
-  <si>
     <t>rebel</t>
   </si>
   <si>
-    <t>%2Fg%2F1225dcz8</t>
-  </si>
-  <si>
     <t>resistance</t>
   </si>
   <si>
-    <t>%2Fm%2F0ld_0</t>
-  </si>
-  <si>
     <t>revolt</t>
   </si>
   <si>
-    <t>%2Fg%2F12215q6f</t>
-  </si>
-  <si>
     <t>riot</t>
   </si>
   <si>
-    <t>%2Fm%2F02k88w</t>
-  </si>
-  <si>
     <t>strike</t>
   </si>
   <si>
-    <t>%2Fm%2F0149p3</t>
-  </si>
-  <si>
     <t>Law and order</t>
   </si>
   <si>
     <t>crime</t>
   </si>
   <si>
-    <t>%2Fg%2F120m10n_</t>
-  </si>
-  <si>
     <t>mafia</t>
   </si>
   <si>
-    <t>%2Fg%2F120t9t47</t>
-  </si>
-  <si>
     <t>police</t>
   </si>
   <si>
-    <t>%2Fm%2F05ws7</t>
-  </si>
-  <si>
     <t>terror</t>
   </si>
   <si>
-    <t>%2Fm%2F0gj940r</t>
-  </si>
-  <si>
     <t>conflict</t>
   </si>
   <si>
-    <t>%2Fm%2F0n5w902</t>
-  </si>
-  <si>
     <t>Tensions</t>
   </si>
   <si>
     <t>discrimination</t>
   </si>
   <si>
-    <t>%2Fm%2F02gg2</t>
-  </si>
-  <si>
     <t>immigration</t>
   </si>
   <si>
-    <t>%2Fm%2F0cbx95</t>
-  </si>
-  <si>
     <t>inequality</t>
   </si>
   <si>
-    <t>%2Fg%2F1221xzk1</t>
-  </si>
-  <si>
     <t>polarization</t>
   </si>
   <si>
-    <t>%2Fm%2F02shm1</t>
-  </si>
-  <si>
     <t>racism</t>
   </si>
   <si>
-    <t>%2Fm%2F06d4h</t>
-  </si>
-  <si>
     <t>tribalism</t>
   </si>
   <si>
-    <t>%2Fm%2F017nbt</t>
-  </si>
-  <si>
     <t>xenophobia</t>
   </si>
   <si>
-    <t>%2Fm%2F08755</t>
-  </si>
-  <si>
     <t>Society</t>
   </si>
   <si>
@@ -693,84 +385,48 @@
     <t>air pollution</t>
   </si>
   <si>
-    <t>%2Fm%2F0dc7h</t>
-  </si>
-  <si>
     <t>water pollution</t>
   </si>
   <si>
-    <t>%2Fm%2F06nzg1</t>
-  </si>
-  <si>
     <t>contamination</t>
   </si>
   <si>
-    <t>%2Fm%2F04jpfyt</t>
-  </si>
-  <si>
     <t>environmental protection</t>
   </si>
   <si>
-    <t>%2Fm%2F04gg7xx</t>
-  </si>
-  <si>
     <t>Soil contamination</t>
   </si>
   <si>
-    <t>%2Fm%2F0br5fz</t>
-  </si>
-  <si>
     <t>Health care</t>
   </si>
   <si>
     <t>health system</t>
   </si>
   <si>
-    <t>%2Fm%2F0gk5f</t>
-  </si>
-  <si>
     <t>health insurance</t>
   </si>
   <si>
-    <t>%2Fm%2F02gqxg</t>
-  </si>
-  <si>
     <t>Social security</t>
   </si>
   <si>
     <t>famine</t>
   </si>
   <si>
-    <t>%2Fm%2F0djn5</t>
-  </si>
-  <si>
     <t>subsidy</t>
   </si>
   <si>
-    <t>%2Fm%2F012qhn</t>
-  </si>
-  <si>
     <t>welfare</t>
   </si>
   <si>
-    <t>%2Fm%2F0968r1</t>
-  </si>
-  <si>
     <t>hunger</t>
   </si>
   <si>
     <t>poverty</t>
   </si>
   <si>
-    <t>%2Fm%2F0h948</t>
-  </si>
-  <si>
     <t>social system</t>
   </si>
   <si>
-    <t>%2Fg%2F1q6jgcr11</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -784,6 +440,339 @@
   </si>
   <si>
     <t>group</t>
+  </si>
+  <si>
+    <t>/m/012_3l</t>
+  </si>
+  <si>
+    <t>/m/0gfps3</t>
+  </si>
+  <si>
+    <t>/g/1211cg58</t>
+  </si>
+  <si>
+    <t>/m/0drqp</t>
+  </si>
+  <si>
+    <t>/m/032qyr</t>
+  </si>
+  <si>
+    <t>/g/120jxn0b</t>
+  </si>
+  <si>
+    <t>/m/013y7y</t>
+  </si>
+  <si>
+    <t>/m/01nnwy</t>
+  </si>
+  <si>
+    <t>/m/0z_xz</t>
+  </si>
+  <si>
+    <t>/m/05q6c7n</t>
+  </si>
+  <si>
+    <t>/m/04g_71</t>
+  </si>
+  <si>
+    <t>/m/04zwh1c</t>
+  </si>
+  <si>
+    <t>/m/07g82</t>
+  </si>
+  <si>
+    <t>/m/01llkn</t>
+  </si>
+  <si>
+    <t>/g/122h6md7</t>
+  </si>
+  <si>
+    <t>/m/0nbdkp6</t>
+  </si>
+  <si>
+    <t>/m/04rsd</t>
+  </si>
+  <si>
+    <t>/m/07s_c</t>
+  </si>
+  <si>
+    <t>/m/04gny</t>
+  </si>
+  <si>
+    <t>/m/01q82</t>
+  </si>
+  <si>
+    <t>/m/01q7l</t>
+  </si>
+  <si>
+    <t>/m/018m33</t>
+  </si>
+  <si>
+    <t>/m/09jx2</t>
+  </si>
+  <si>
+    <t>/m/04n7dpf</t>
+  </si>
+  <si>
+    <t>/m/01rd35</t>
+  </si>
+  <si>
+    <t>/m/016ldw</t>
+  </si>
+  <si>
+    <t>/m/01l28h</t>
+  </si>
+  <si>
+    <t>/g/121rjn4x</t>
+  </si>
+  <si>
+    <t>/m/04rdmz</t>
+  </si>
+  <si>
+    <t>/m/0mxcs</t>
+  </si>
+  <si>
+    <t>/m/0h6sm4</t>
+  </si>
+  <si>
+    <t>/m/05lkwy</t>
+  </si>
+  <si>
+    <t>/m/04rwd</t>
+  </si>
+  <si>
+    <t>/m/05sq5</t>
+  </si>
+  <si>
+    <t>/m/0mxd7</t>
+  </si>
+  <si>
+    <t>/m/013zzb</t>
+  </si>
+  <si>
+    <t>/m/013z93</t>
+  </si>
+  <si>
+    <t>/m/0ffnx</t>
+  </si>
+  <si>
+    <t>/m/0bhbmdc</t>
+  </si>
+  <si>
+    <t>/m/01fsk5</t>
+  </si>
+  <si>
+    <t>/m/014zf</t>
+  </si>
+  <si>
+    <t>/m/0d8tn</t>
+  </si>
+  <si>
+    <t>/m/02bms</t>
+  </si>
+  <si>
+    <t>/m/02zmm</t>
+  </si>
+  <si>
+    <t>/g/11c5s_rnxq</t>
+  </si>
+  <si>
+    <t>/m/04qwqn</t>
+  </si>
+  <si>
+    <t>/m/099cd</t>
+  </si>
+  <si>
+    <t>/m/017tz9</t>
+  </si>
+  <si>
+    <t>/m/01mq8p</t>
+  </si>
+  <si>
+    <t>/m/01g_y</t>
+  </si>
+  <si>
+    <t>/m/09pngm</t>
+  </si>
+  <si>
+    <t>/m/01tj9r</t>
+  </si>
+  <si>
+    <t>/m/036nz</t>
+  </si>
+  <si>
+    <t>/m/05_5d</t>
+  </si>
+  <si>
+    <t>/m/05qt0</t>
+  </si>
+  <si>
+    <t>/m/0127bq</t>
+  </si>
+  <si>
+    <t>/m/0k05r</t>
+  </si>
+  <si>
+    <t>/m/042px7</t>
+  </si>
+  <si>
+    <t>/m/02wwvy</t>
+  </si>
+  <si>
+    <t>/m/025k7</t>
+  </si>
+  <si>
+    <t>/m/02l3h</t>
+  </si>
+  <si>
+    <t>/m/03yr9</t>
+  </si>
+  <si>
+    <t>/m/098j6v</t>
+  </si>
+  <si>
+    <t>/m/0pgkc</t>
+  </si>
+  <si>
+    <t>/m/01h6rj</t>
+  </si>
+  <si>
+    <t>/m/01qvj2</t>
+  </si>
+  <si>
+    <t>/g/1218dzhd</t>
+  </si>
+  <si>
+    <t>/g/1q6j9fx10</t>
+  </si>
+  <si>
+    <t>/m/06mz9c</t>
+  </si>
+  <si>
+    <t>/m/082cb</t>
+  </si>
+  <si>
+    <t>/m/032b8</t>
+  </si>
+  <si>
+    <t>/m/0gwb1</t>
+  </si>
+  <si>
+    <t>/m/0dbs_</t>
+  </si>
+  <si>
+    <t>/m/055sg</t>
+  </si>
+  <si>
+    <t>/g/120ry1nd</t>
+  </si>
+  <si>
+    <t>/g/1225dcz8</t>
+  </si>
+  <si>
+    <t>/m/0ld_0</t>
+  </si>
+  <si>
+    <t>/g/12215q6f</t>
+  </si>
+  <si>
+    <t>/m/02k88w</t>
+  </si>
+  <si>
+    <t>/m/0149p3</t>
+  </si>
+  <si>
+    <t>/m/0gj940r</t>
+  </si>
+  <si>
+    <t>/g/120m10n_</t>
+  </si>
+  <si>
+    <t>/g/120t9t47</t>
+  </si>
+  <si>
+    <t>/m/05ws7</t>
+  </si>
+  <si>
+    <t>/m/0n5w902</t>
+  </si>
+  <si>
+    <t>/m/02gg2</t>
+  </si>
+  <si>
+    <t>/m/0cbx95</t>
+  </si>
+  <si>
+    <t>/g/1221xzk1</t>
+  </si>
+  <si>
+    <t>/m/02shm1</t>
+  </si>
+  <si>
+    <t>/m/06d4h</t>
+  </si>
+  <si>
+    <t>/m/017nbt</t>
+  </si>
+  <si>
+    <t>/m/08755</t>
+  </si>
+  <si>
+    <t>/m/0dc7h</t>
+  </si>
+  <si>
+    <t>/m/06nzg1</t>
+  </si>
+  <si>
+    <t>/m/04jpfyt</t>
+  </si>
+  <si>
+    <t>/m/04_wkd</t>
+  </si>
+  <si>
+    <t>/m/04gg7xx</t>
+  </si>
+  <si>
+    <t>/m/0br5fz</t>
+  </si>
+  <si>
+    <t>/m/0gk5f</t>
+  </si>
+  <si>
+    <t>/m/02gqxg</t>
+  </si>
+  <si>
+    <t>/m/0djn5</t>
+  </si>
+  <si>
+    <t>/m/012qhn</t>
+  </si>
+  <si>
+    <t>/m/0968r1</t>
+  </si>
+  <si>
+    <t>/m/0h948</t>
+  </si>
+  <si>
+    <t>/g/1q6jgcr11</t>
+  </si>
+  <si>
+    <t>/g/121zc50z</t>
+  </si>
+  <si>
+    <t>/m/02q_bk</t>
+  </si>
+  <si>
+    <t>/m/055t58</t>
+  </si>
+  <si>
+    <t>/m/025sndk</t>
+  </si>
+  <si>
+    <t>/m/0d07ph</t>
+  </si>
+  <si>
+    <t>/m/09jcvs</t>
   </si>
 </sst>
 </file>
@@ -1137,22 +1126,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87F390F-A2A5-468A-9188-7F795F2C1C7F}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
-        <v>244</v>
+        <v>133</v>
       </c>
       <c r="C1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1160,10 +1149,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1171,10 +1160,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1182,10 +1171,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1193,10 +1182,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1204,7 +1193,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -1216,1850 +1205,1851 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDC686DA-856D-4AE4-86F6-93767FAF2C3B}">
   <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83:XFD83"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
-        <v>246</v>
+        <v>135</v>
       </c>
       <c r="C1" t="s">
-        <v>247</v>
+        <v>136</v>
       </c>
       <c r="D1" t="s">
-        <v>244</v>
+        <v>133</v>
       </c>
       <c r="E1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
       <c r="E2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
         <v>26</v>
       </c>
-      <c r="D14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" t="s">
-        <v>48</v>
-      </c>
       <c r="E16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="E20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="E21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="E24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="E25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="E26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="D27" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="E27" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="E28" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="D29" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="E29" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="D30" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="E30" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="E31" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="E32" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="D33" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="E33" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>10</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="E34" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="D35" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E35" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="D36" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="E36" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="D37" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="E37" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="D38" t="s">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="E38" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="D39" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="E39" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="D40" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E40" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="D41" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="E41" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
       <c r="D42" t="s">
-        <v>104</v>
+        <v>56</v>
       </c>
       <c r="E42" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C43" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
       <c r="D43" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="E43" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C44" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
       <c r="D44" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="E44" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>13</v>
       </c>
       <c r="B45" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C45" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
       <c r="D45" t="s">
-        <v>110</v>
+        <v>59</v>
       </c>
       <c r="E45" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>14</v>
       </c>
       <c r="B46" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C46" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
       <c r="D46" t="s">
-        <v>112</v>
+        <v>60</v>
       </c>
       <c r="E46" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C47" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
       <c r="D47" t="s">
-        <v>114</v>
+        <v>61</v>
       </c>
       <c r="E47" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>14</v>
       </c>
       <c r="B48" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C48" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
       <c r="D48" t="s">
-        <v>116</v>
+        <v>62</v>
       </c>
       <c r="E48" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>14</v>
       </c>
       <c r="B49" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C49" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
       <c r="D49" t="s">
-        <v>118</v>
+        <v>63</v>
       </c>
       <c r="E49" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>15</v>
       </c>
       <c r="B50" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C50" t="s">
-        <v>120</v>
+        <v>64</v>
       </c>
       <c r="D50" t="s">
-        <v>121</v>
+        <v>65</v>
       </c>
       <c r="E50" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>120</v>
+        <v>64</v>
       </c>
       <c r="D51" t="s">
-        <v>123</v>
+        <v>66</v>
       </c>
       <c r="E51" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C52" t="s">
-        <v>120</v>
+        <v>64</v>
       </c>
       <c r="D52" t="s">
-        <v>125</v>
+        <v>67</v>
       </c>
       <c r="E52" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C53" t="s">
-        <v>120</v>
+        <v>64</v>
       </c>
       <c r="D53" t="s">
-        <v>138</v>
+        <v>74</v>
       </c>
       <c r="E53" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>16</v>
       </c>
       <c r="B54" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C54" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="D54" t="s">
-        <v>129</v>
+        <v>69</v>
       </c>
       <c r="E54" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>16</v>
       </c>
       <c r="B55" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="D55" t="s">
-        <v>131</v>
+        <v>70</v>
       </c>
       <c r="E55" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="D56" t="s">
-        <v>133</v>
+        <v>71</v>
       </c>
       <c r="E56" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C57" t="s">
-        <v>135</v>
+        <v>72</v>
       </c>
       <c r="D57" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E57" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C58" t="s">
-        <v>135</v>
+        <v>72</v>
       </c>
       <c r="D58" t="s">
-        <v>136</v>
+        <v>73</v>
       </c>
       <c r="E58" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>17</v>
       </c>
       <c r="B59" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C59" t="s">
-        <v>135</v>
+        <v>72</v>
       </c>
       <c r="D59" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E59" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>18</v>
       </c>
       <c r="B60" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C60" t="s">
-        <v>140</v>
+        <v>75</v>
       </c>
       <c r="D60" t="s">
-        <v>141</v>
+        <v>76</v>
       </c>
       <c r="E60" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>18</v>
       </c>
       <c r="B61" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C61" t="s">
-        <v>140</v>
+        <v>75</v>
       </c>
       <c r="D61" t="s">
-        <v>143</v>
+        <v>77</v>
       </c>
       <c r="E61" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>18</v>
       </c>
       <c r="B62" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C62" t="s">
-        <v>140</v>
+        <v>75</v>
       </c>
       <c r="D62" t="s">
-        <v>145</v>
+        <v>78</v>
       </c>
       <c r="E62" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>18</v>
       </c>
       <c r="B63" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C63" t="s">
-        <v>140</v>
+        <v>75</v>
       </c>
       <c r="D63" t="s">
-        <v>147</v>
+        <v>79</v>
       </c>
       <c r="E63" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>19</v>
       </c>
       <c r="B64" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C64" t="s">
-        <v>140</v>
+        <v>75</v>
       </c>
       <c r="D64" t="s">
-        <v>149</v>
+        <v>80</v>
       </c>
       <c r="E64" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>19</v>
       </c>
       <c r="B65" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C65" t="s">
-        <v>140</v>
+        <v>75</v>
       </c>
       <c r="D65" t="s">
-        <v>151</v>
+        <v>81</v>
       </c>
       <c r="E65" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>20</v>
       </c>
       <c r="B66" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C66" t="s">
-        <v>154</v>
+        <v>83</v>
       </c>
       <c r="D66" t="s">
-        <v>155</v>
+        <v>84</v>
       </c>
       <c r="E66" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>20</v>
       </c>
       <c r="B67" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C67" t="s">
-        <v>154</v>
+        <v>83</v>
       </c>
       <c r="D67" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
       <c r="E67" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>20</v>
       </c>
       <c r="B68" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C68" t="s">
-        <v>154</v>
+        <v>83</v>
       </c>
       <c r="D68" t="s">
-        <v>159</v>
+        <v>86</v>
       </c>
       <c r="E68" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>20</v>
       </c>
       <c r="B69" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C69" t="s">
-        <v>154</v>
+        <v>83</v>
       </c>
       <c r="D69" t="s">
-        <v>161</v>
+        <v>87</v>
       </c>
       <c r="E69" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>21</v>
       </c>
       <c r="B70" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C70" t="s">
-        <v>154</v>
+        <v>83</v>
       </c>
       <c r="D70" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="E70" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>21</v>
       </c>
       <c r="B71" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C71" t="s">
-        <v>154</v>
+        <v>83</v>
       </c>
       <c r="D71" t="s">
-        <v>165</v>
+        <v>89</v>
       </c>
       <c r="E71" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>22</v>
       </c>
       <c r="B72" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C72" t="s">
-        <v>167</v>
+        <v>90</v>
       </c>
       <c r="D72" t="s">
-        <v>168</v>
+        <v>91</v>
       </c>
       <c r="E72" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>22</v>
       </c>
       <c r="B73" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C73" t="s">
-        <v>167</v>
+        <v>90</v>
       </c>
       <c r="D73" t="s">
-        <v>170</v>
+        <v>92</v>
       </c>
       <c r="E73" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>22</v>
       </c>
       <c r="B74" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C74" t="s">
-        <v>167</v>
+        <v>90</v>
       </c>
       <c r="D74" t="s">
-        <v>172</v>
+        <v>93</v>
       </c>
       <c r="E74" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>22</v>
       </c>
       <c r="B75" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C75" t="s">
-        <v>167</v>
+        <v>90</v>
       </c>
       <c r="D75" t="s">
-        <v>174</v>
+        <v>94</v>
       </c>
       <c r="E75" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>23</v>
       </c>
       <c r="B76" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C76" t="s">
-        <v>167</v>
+        <v>90</v>
       </c>
       <c r="D76" t="s">
-        <v>176</v>
+        <v>95</v>
       </c>
       <c r="E76" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>23</v>
       </c>
       <c r="B77" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C77" t="s">
-        <v>167</v>
+        <v>90</v>
       </c>
       <c r="D77" t="s">
-        <v>178</v>
+        <v>96</v>
       </c>
       <c r="E77" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>23</v>
       </c>
       <c r="B78" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C78" t="s">
-        <v>167</v>
+        <v>90</v>
       </c>
       <c r="D78" t="s">
-        <v>180</v>
+        <v>97</v>
       </c>
       <c r="E78" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>23</v>
       </c>
       <c r="B79" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C79" t="s">
-        <v>167</v>
+        <v>90</v>
       </c>
       <c r="D79" t="s">
-        <v>182</v>
+        <v>98</v>
       </c>
       <c r="E79" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>24</v>
       </c>
       <c r="B80" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C80" t="s">
-        <v>167</v>
+        <v>90</v>
       </c>
       <c r="D80" t="s">
-        <v>184</v>
+        <v>99</v>
       </c>
       <c r="E80" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>24</v>
       </c>
       <c r="B81" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C81" t="s">
-        <v>167</v>
+        <v>90</v>
       </c>
       <c r="D81" t="s">
-        <v>186</v>
+        <v>100</v>
       </c>
       <c r="E81" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>24</v>
       </c>
       <c r="B82" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C82" t="s">
-        <v>167</v>
+        <v>90</v>
       </c>
       <c r="D82" t="s">
-        <v>195</v>
+        <v>105</v>
       </c>
       <c r="E82" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>25</v>
       </c>
       <c r="B83" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C83" t="s">
-        <v>188</v>
+        <v>101</v>
       </c>
       <c r="D83" t="s">
-        <v>189</v>
+        <v>102</v>
       </c>
       <c r="E83" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>25</v>
       </c>
       <c r="B84" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C84" t="s">
-        <v>188</v>
+        <v>101</v>
       </c>
       <c r="D84" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="E84" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>25</v>
       </c>
       <c r="B85" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C85" t="s">
-        <v>188</v>
+        <v>101</v>
       </c>
       <c r="D85" t="s">
-        <v>193</v>
+        <v>104</v>
       </c>
       <c r="E85" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>26</v>
       </c>
       <c r="B86" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C86" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="D86" t="s">
-        <v>197</v>
+        <v>106</v>
       </c>
       <c r="E86" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>27</v>
       </c>
       <c r="B87" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C87" t="s">
-        <v>199</v>
+        <v>107</v>
       </c>
       <c r="D87" t="s">
-        <v>200</v>
+        <v>108</v>
       </c>
       <c r="E87" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>27</v>
       </c>
       <c r="B88" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C88" t="s">
-        <v>199</v>
+        <v>107</v>
       </c>
       <c r="D88" t="s">
-        <v>202</v>
+        <v>109</v>
       </c>
       <c r="E88" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>27</v>
       </c>
       <c r="B89" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C89" t="s">
-        <v>199</v>
+        <v>107</v>
       </c>
       <c r="D89" t="s">
-        <v>204</v>
+        <v>110</v>
       </c>
       <c r="E89" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>27</v>
       </c>
       <c r="B90" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C90" t="s">
-        <v>199</v>
+        <v>107</v>
       </c>
       <c r="D90" t="s">
-        <v>206</v>
+        <v>111</v>
       </c>
       <c r="E90" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>28</v>
       </c>
       <c r="B91" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C91" t="s">
-        <v>199</v>
+        <v>107</v>
       </c>
       <c r="D91" t="s">
-        <v>208</v>
+        <v>112</v>
       </c>
       <c r="E91" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>28</v>
       </c>
       <c r="B92" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C92" t="s">
-        <v>199</v>
+        <v>107</v>
       </c>
       <c r="D92" t="s">
-        <v>210</v>
+        <v>113</v>
       </c>
       <c r="E92" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>28</v>
       </c>
       <c r="B93" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="C93" t="s">
-        <v>199</v>
+        <v>107</v>
       </c>
       <c r="D93" t="s">
-        <v>212</v>
+        <v>114</v>
       </c>
       <c r="E93" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>29</v>
       </c>
       <c r="B94" t="s">
-        <v>214</v>
+        <v>115</v>
       </c>
       <c r="C94" t="s">
-        <v>215</v>
+        <v>116</v>
       </c>
       <c r="D94" t="s">
-        <v>216</v>
+        <v>117</v>
       </c>
       <c r="E94" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>29</v>
       </c>
       <c r="B95" t="s">
-        <v>214</v>
+        <v>115</v>
       </c>
       <c r="C95" t="s">
-        <v>215</v>
+        <v>116</v>
       </c>
       <c r="D95" t="s">
-        <v>218</v>
+        <v>118</v>
       </c>
       <c r="E95" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>29</v>
       </c>
       <c r="B96" t="s">
-        <v>214</v>
+        <v>115</v>
       </c>
       <c r="C96" t="s">
-        <v>215</v>
+        <v>116</v>
       </c>
       <c r="D96" t="s">
-        <v>220</v>
+        <v>119</v>
       </c>
       <c r="E96" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>29</v>
       </c>
       <c r="B97" t="s">
-        <v>214</v>
+        <v>115</v>
       </c>
       <c r="C97" t="s">
-        <v>215</v>
+        <v>116</v>
       </c>
       <c r="D97" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E97" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>30</v>
       </c>
       <c r="B98" t="s">
-        <v>214</v>
+        <v>115</v>
       </c>
       <c r="C98" t="s">
-        <v>215</v>
+        <v>116</v>
       </c>
       <c r="D98" t="s">
-        <v>222</v>
+        <v>120</v>
       </c>
       <c r="E98" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>30</v>
       </c>
       <c r="B99" t="s">
-        <v>214</v>
+        <v>115</v>
       </c>
       <c r="C99" t="s">
-        <v>215</v>
+        <v>116</v>
       </c>
       <c r="D99" t="s">
-        <v>224</v>
+        <v>121</v>
       </c>
       <c r="E99" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>31</v>
       </c>
       <c r="B100" t="s">
-        <v>214</v>
+        <v>115</v>
       </c>
       <c r="C100" t="s">
-        <v>226</v>
+        <v>122</v>
       </c>
       <c r="D100" t="s">
-        <v>227</v>
+        <v>123</v>
       </c>
       <c r="E100" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>31</v>
       </c>
       <c r="B101" t="s">
-        <v>214</v>
+        <v>115</v>
       </c>
       <c r="C101" t="s">
-        <v>226</v>
+        <v>122</v>
       </c>
       <c r="D101" t="s">
-        <v>229</v>
+        <v>124</v>
       </c>
       <c r="E101" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>31</v>
       </c>
       <c r="B102" t="s">
-        <v>214</v>
+        <v>115</v>
       </c>
       <c r="C102" t="s">
-        <v>231</v>
+        <v>125</v>
       </c>
       <c r="D102" t="s">
-        <v>232</v>
+        <v>126</v>
       </c>
       <c r="E102" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>31</v>
       </c>
       <c r="B103" t="s">
-        <v>214</v>
+        <v>115</v>
       </c>
       <c r="C103" t="s">
-        <v>231</v>
+        <v>125</v>
       </c>
       <c r="D103" t="s">
-        <v>234</v>
+        <v>127</v>
       </c>
       <c r="E103" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>32</v>
       </c>
       <c r="B104" t="s">
-        <v>214</v>
+        <v>115</v>
       </c>
       <c r="C104" t="s">
-        <v>231</v>
+        <v>125</v>
       </c>
       <c r="D104" t="s">
-        <v>236</v>
+        <v>128</v>
       </c>
       <c r="E104" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>32</v>
       </c>
       <c r="B105" t="s">
-        <v>214</v>
+        <v>115</v>
       </c>
       <c r="C105" t="s">
-        <v>231</v>
+        <v>125</v>
       </c>
       <c r="D105" t="s">
-        <v>238</v>
+        <v>129</v>
       </c>
       <c r="E105" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>32</v>
       </c>
       <c r="B106" t="s">
-        <v>214</v>
+        <v>115</v>
       </c>
       <c r="C106" t="s">
-        <v>231</v>
+        <v>125</v>
       </c>
       <c r="D106" t="s">
-        <v>239</v>
+        <v>130</v>
       </c>
       <c r="E106" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>32</v>
       </c>
       <c r="B107" t="s">
-        <v>214</v>
+        <v>115</v>
       </c>
       <c r="C107" t="s">
-        <v>231</v>
+        <v>125</v>
       </c>
       <c r="D107" t="s">
+        <v>131</v>
+      </c>
+      <c r="E107" t="s">
         <v>241</v>
       </c>
-      <c r="E107" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>33</v>
       </c>
       <c r="B108" t="s">
-        <v>214</v>
+        <v>115</v>
       </c>
       <c r="C108" t="s">
-        <v>231</v>
+        <v>125</v>
       </c>
       <c r="D108" t="s">
-        <v>127</v>
+        <v>68</v>
       </c>
       <c r="E108" t="s">
-        <v>128</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B1:E108" xr:uid="{EB268C2C-A3FE-47C3-8EC4-86AD6D2407C4}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove famine double count
</commit_message>
<xml_diff>
--- a/input/spri_topics.xlsx
+++ b/input/spri_topics.xlsx
@@ -1,35 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c4361369\Documents\GitHub\globaltrends_spri\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haral\Dropbox\Data\globaltrends_spri\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D223D7B4-DAD0-4F94-B47D-2375E48934FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBED9FB-5BB1-4858-A22F-EC5424E7A3F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="20712" windowHeight="13512" xr2:uid="{10DCA323-7FCA-4127-8054-0B27B40AD918}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{10DCA323-7FCA-4127-8054-0B27B40AD918}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tabelle2!$B$1:$E$108</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tabelle2!$B$1:$E$107</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="247">
   <si>
     <t>Gmail</t>
   </si>
@@ -407,9 +418,6 @@
   </si>
   <si>
     <t>Social security</t>
-  </si>
-  <si>
-    <t>famine</t>
   </si>
   <si>
     <t>subsidy</t>
@@ -828,9 +836,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -868,7 +876,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -974,7 +982,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1116,7 +1124,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1126,22 +1134,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87F390F-A2A5-468A-9188-7F795F2C1C7F}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" t="s">
         <v>132</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>133</v>
       </c>
-      <c r="C1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1149,10 +1157,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1160,10 +1168,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1171,10 +1179,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1182,10 +1190,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1193,7 +1201,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -1203,32 +1211,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDC686DA-856D-4AE4-86F6-93767FAF2C3B}">
-  <dimension ref="A1:E108"/>
+  <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E108"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" t="s">
         <v>132</v>
       </c>
-      <c r="B1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>133</v>
       </c>
-      <c r="E1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1242,10 +1248,10 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1259,10 +1265,10 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1276,10 +1282,10 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1293,10 +1299,10 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1310,10 +1316,10 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1327,10 +1333,10 @@
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1344,10 +1350,10 @@
         <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1361,10 +1367,10 @@
         <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1378,10 +1384,10 @@
         <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1395,10 +1401,10 @@
         <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1412,10 +1418,10 @@
         <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1429,10 +1435,10 @@
         <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1446,10 +1452,10 @@
         <v>23</v>
       </c>
       <c r="E14" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1463,10 +1469,10 @@
         <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1480,10 +1486,10 @@
         <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>5</v>
       </c>
@@ -1497,10 +1503,10 @@
         <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>5</v>
       </c>
@@ -1514,10 +1520,10 @@
         <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>6</v>
       </c>
@@ -1531,10 +1537,10 @@
         <v>29</v>
       </c>
       <c r="E19" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>6</v>
       </c>
@@ -1548,10 +1554,10 @@
         <v>30</v>
       </c>
       <c r="E20" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>7</v>
       </c>
@@ -1565,10 +1571,10 @@
         <v>32</v>
       </c>
       <c r="E21" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>7</v>
       </c>
@@ -1582,10 +1588,10 @@
         <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>7</v>
       </c>
@@ -1599,10 +1605,10 @@
         <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>7</v>
       </c>
@@ -1616,10 +1622,10 @@
         <v>35</v>
       </c>
       <c r="E24" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>8</v>
       </c>
@@ -1633,10 +1639,10 @@
         <v>36</v>
       </c>
       <c r="E25" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>8</v>
       </c>
@@ -1650,10 +1656,10 @@
         <v>37</v>
       </c>
       <c r="E26" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>8</v>
       </c>
@@ -1667,10 +1673,10 @@
         <v>38</v>
       </c>
       <c r="E27" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>9</v>
       </c>
@@ -1684,10 +1690,10 @@
         <v>40</v>
       </c>
       <c r="E28" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>9</v>
       </c>
@@ -1701,10 +1707,10 @@
         <v>41</v>
       </c>
       <c r="E29" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>9</v>
       </c>
@@ -1718,10 +1724,10 @@
         <v>42</v>
       </c>
       <c r="E30" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>9</v>
       </c>
@@ -1735,10 +1741,10 @@
         <v>43</v>
       </c>
       <c r="E31" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>10</v>
       </c>
@@ -1752,10 +1758,10 @@
         <v>44</v>
       </c>
       <c r="E32" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>10</v>
       </c>
@@ -1769,10 +1775,10 @@
         <v>45</v>
       </c>
       <c r="E33" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>10</v>
       </c>
@@ -1786,10 +1792,10 @@
         <v>46</v>
       </c>
       <c r="E34" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>10</v>
       </c>
@@ -1803,10 +1809,10 @@
         <v>47</v>
       </c>
       <c r="E35" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>11</v>
       </c>
@@ -1820,10 +1826,10 @@
         <v>48</v>
       </c>
       <c r="E36" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>11</v>
       </c>
@@ -1837,10 +1843,10 @@
         <v>49</v>
       </c>
       <c r="E37" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>12</v>
       </c>
@@ -1854,10 +1860,10 @@
         <v>51</v>
       </c>
       <c r="E38" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>12</v>
       </c>
@@ -1871,10 +1877,10 @@
         <v>52</v>
       </c>
       <c r="E39" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>12</v>
       </c>
@@ -1888,10 +1894,10 @@
         <v>9</v>
       </c>
       <c r="E40" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>12</v>
       </c>
@@ -1905,10 +1911,10 @@
         <v>53</v>
       </c>
       <c r="E41" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>13</v>
       </c>
@@ -1922,10 +1928,10 @@
         <v>56</v>
       </c>
       <c r="E42" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>13</v>
       </c>
@@ -1939,10 +1945,10 @@
         <v>57</v>
       </c>
       <c r="E43" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>13</v>
       </c>
@@ -1956,10 +1962,10 @@
         <v>58</v>
       </c>
       <c r="E44" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>13</v>
       </c>
@@ -1973,10 +1979,10 @@
         <v>59</v>
       </c>
       <c r="E45" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>14</v>
       </c>
@@ -1990,10 +1996,10 @@
         <v>60</v>
       </c>
       <c r="E46" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>14</v>
       </c>
@@ -2007,10 +2013,10 @@
         <v>61</v>
       </c>
       <c r="E47" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>14</v>
       </c>
@@ -2024,10 +2030,10 @@
         <v>62</v>
       </c>
       <c r="E48" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>14</v>
       </c>
@@ -2041,10 +2047,10 @@
         <v>63</v>
       </c>
       <c r="E49" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>15</v>
       </c>
@@ -2058,10 +2064,10 @@
         <v>65</v>
       </c>
       <c r="E50" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>15</v>
       </c>
@@ -2075,10 +2081,10 @@
         <v>66</v>
       </c>
       <c r="E51" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>15</v>
       </c>
@@ -2092,10 +2098,10 @@
         <v>67</v>
       </c>
       <c r="E52" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>15</v>
       </c>
@@ -2109,10 +2115,10 @@
         <v>74</v>
       </c>
       <c r="E53" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>16</v>
       </c>
@@ -2126,10 +2132,10 @@
         <v>69</v>
       </c>
       <c r="E54" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>16</v>
       </c>
@@ -2143,10 +2149,10 @@
         <v>70</v>
       </c>
       <c r="E55" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>16</v>
       </c>
@@ -2160,10 +2166,10 @@
         <v>71</v>
       </c>
       <c r="E56" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>17</v>
       </c>
@@ -2177,10 +2183,10 @@
         <v>7</v>
       </c>
       <c r="E57" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>17</v>
       </c>
@@ -2194,10 +2200,10 @@
         <v>73</v>
       </c>
       <c r="E58" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>17</v>
       </c>
@@ -2211,10 +2217,10 @@
         <v>8</v>
       </c>
       <c r="E59" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>18</v>
       </c>
@@ -2228,10 +2234,10 @@
         <v>76</v>
       </c>
       <c r="E60" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>18</v>
       </c>
@@ -2245,10 +2251,10 @@
         <v>77</v>
       </c>
       <c r="E61" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>18</v>
       </c>
@@ -2262,10 +2268,10 @@
         <v>78</v>
       </c>
       <c r="E62" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>18</v>
       </c>
@@ -2279,10 +2285,10 @@
         <v>79</v>
       </c>
       <c r="E63" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>19</v>
       </c>
@@ -2296,10 +2302,10 @@
         <v>80</v>
       </c>
       <c r="E64" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>19</v>
       </c>
@@ -2313,10 +2319,10 @@
         <v>81</v>
       </c>
       <c r="E65" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>20</v>
       </c>
@@ -2330,10 +2336,10 @@
         <v>84</v>
       </c>
       <c r="E66" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>20</v>
       </c>
@@ -2347,10 +2353,10 @@
         <v>85</v>
       </c>
       <c r="E67" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>20</v>
       </c>
@@ -2364,10 +2370,10 @@
         <v>86</v>
       </c>
       <c r="E68" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>20</v>
       </c>
@@ -2381,10 +2387,10 @@
         <v>87</v>
       </c>
       <c r="E69" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>21</v>
       </c>
@@ -2398,10 +2404,10 @@
         <v>88</v>
       </c>
       <c r="E70" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>21</v>
       </c>
@@ -2415,10 +2421,10 @@
         <v>89</v>
       </c>
       <c r="E71" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>22</v>
       </c>
@@ -2432,10 +2438,10 @@
         <v>91</v>
       </c>
       <c r="E72" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>22</v>
       </c>
@@ -2449,10 +2455,10 @@
         <v>92</v>
       </c>
       <c r="E73" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>22</v>
       </c>
@@ -2466,10 +2472,10 @@
         <v>93</v>
       </c>
       <c r="E74" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>22</v>
       </c>
@@ -2483,10 +2489,10 @@
         <v>94</v>
       </c>
       <c r="E75" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>23</v>
       </c>
@@ -2500,10 +2506,10 @@
         <v>95</v>
       </c>
       <c r="E76" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>23</v>
       </c>
@@ -2517,10 +2523,10 @@
         <v>96</v>
       </c>
       <c r="E77" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>23</v>
       </c>
@@ -2534,10 +2540,10 @@
         <v>97</v>
       </c>
       <c r="E78" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>23</v>
       </c>
@@ -2551,10 +2557,10 @@
         <v>98</v>
       </c>
       <c r="E79" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>24</v>
       </c>
@@ -2568,10 +2574,10 @@
         <v>99</v>
       </c>
       <c r="E80" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>24</v>
       </c>
@@ -2585,10 +2591,10 @@
         <v>100</v>
       </c>
       <c r="E81" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>24</v>
       </c>
@@ -2602,10 +2608,10 @@
         <v>105</v>
       </c>
       <c r="E82" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>25</v>
       </c>
@@ -2619,10 +2625,10 @@
         <v>102</v>
       </c>
       <c r="E83" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>25</v>
       </c>
@@ -2636,10 +2642,10 @@
         <v>103</v>
       </c>
       <c r="E84" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>25</v>
       </c>
@@ -2653,10 +2659,10 @@
         <v>104</v>
       </c>
       <c r="E85" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>26</v>
       </c>
@@ -2670,10 +2676,10 @@
         <v>106</v>
       </c>
       <c r="E86" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>27</v>
       </c>
@@ -2687,10 +2693,10 @@
         <v>108</v>
       </c>
       <c r="E87" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>27</v>
       </c>
@@ -2704,10 +2710,10 @@
         <v>109</v>
       </c>
       <c r="E88" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>27</v>
       </c>
@@ -2721,10 +2727,10 @@
         <v>110</v>
       </c>
       <c r="E89" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>27</v>
       </c>
@@ -2738,10 +2744,10 @@
         <v>111</v>
       </c>
       <c r="E90" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>28</v>
       </c>
@@ -2755,10 +2761,10 @@
         <v>112</v>
       </c>
       <c r="E91" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>28</v>
       </c>
@@ -2772,10 +2778,10 @@
         <v>113</v>
       </c>
       <c r="E92" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>28</v>
       </c>
@@ -2789,10 +2795,10 @@
         <v>114</v>
       </c>
       <c r="E93" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>29</v>
       </c>
@@ -2806,10 +2812,10 @@
         <v>117</v>
       </c>
       <c r="E94" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>29</v>
       </c>
@@ -2823,10 +2829,10 @@
         <v>118</v>
       </c>
       <c r="E95" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>29</v>
       </c>
@@ -2840,10 +2846,10 @@
         <v>119</v>
       </c>
       <c r="E96" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>29</v>
       </c>
@@ -2857,10 +2863,10 @@
         <v>6</v>
       </c>
       <c r="E97" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>30</v>
       </c>
@@ -2874,10 +2880,10 @@
         <v>120</v>
       </c>
       <c r="E98" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>30</v>
       </c>
@@ -2891,10 +2897,10 @@
         <v>121</v>
       </c>
       <c r="E99" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>31</v>
       </c>
@@ -2908,10 +2914,10 @@
         <v>123</v>
       </c>
       <c r="E100" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>31</v>
       </c>
@@ -2925,10 +2931,10 @@
         <v>124</v>
       </c>
       <c r="E101" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>31</v>
       </c>
@@ -2945,9 +2951,9 @@
         <v>237</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B103" t="s">
         <v>115</v>
@@ -2962,7 +2968,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>32</v>
       </c>
@@ -2976,10 +2982,10 @@
         <v>128</v>
       </c>
       <c r="E104" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>32</v>
       </c>
@@ -2993,10 +2999,10 @@
         <v>129</v>
       </c>
       <c r="E105" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>32</v>
       </c>
@@ -3013,9 +3019,9 @@
         <v>240</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B107" t="s">
         <v>115</v>
@@ -3024,31 +3030,14 @@
         <v>125</v>
       </c>
       <c r="D107" t="s">
-        <v>131</v>
+        <v>68</v>
       </c>
       <c r="E107" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A108">
-        <v>33</v>
-      </c>
-      <c r="B108" t="s">
-        <v>115</v>
-      </c>
-      <c r="C108" t="s">
-        <v>125</v>
-      </c>
-      <c r="D108" t="s">
-        <v>68</v>
-      </c>
-      <c r="E108" t="s">
-        <v>242</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="B1:E108" xr:uid="{EB268C2C-A3FE-47C3-8EC4-86AD6D2407C4}"/>
+  <autoFilter ref="B1:E107" xr:uid="{EB268C2C-A3FE-47C3-8EC4-86AD6D2407C4}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>